<commit_message>
Se agrego dato logico
</commit_message>
<xml_diff>
--- a/autoventa.XLSX
+++ b/autoventa.XLSX
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrique.artero\OneDrive - Productos Alimenticios Diana, S.A. de C.V\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\python-leer-excel-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6717F0-C359-4858-93A4-D9112D1DE51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picking Autoventa" sheetId="1" r:id="rId1"/>
@@ -194,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -252,11 +253,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -538,12 +538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
@@ -552,714 +554,714 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>11001</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>54</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>11003</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>11007</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>11009</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>11038</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>11099</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>11137</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>11154</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>11489</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>11558</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>11560</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>11647</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>11649</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>11654</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>24</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>11655</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>12</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>11656</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>11664</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>11665</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>11795</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="1">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>11806</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>11808</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>11867</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>5</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>11974</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>11978</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>11993</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>11994</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="1">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>11996</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="1">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>12003</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>110</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>12008</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>60</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>12019</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>100</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>12035</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>360</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>12037</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>160</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>12038</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>300</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>12039</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>180</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>12040</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="1">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>12041</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="1">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>12042</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="1">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
         <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>12058</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>70</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>12062</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="1">
-        <v>4</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>12063</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>10</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>12064</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43">
         <v>12086</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
         <v>8</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44">
         <v>12088</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>8</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45">
         <v>12089</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>10</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46">
         <v>12090</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="1">
-        <v>6</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
         <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47">
         <v>12131</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>15</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47">
         <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48">
         <v>12132</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>15</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49">
         <v>12177</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>55</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49">
         <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50">
         <v>12217</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
         <v>8</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
se Termito la parte del umb
</commit_message>
<xml_diff>
--- a/autoventa.XLSX
+++ b/autoventa.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\python-leer-excel-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63B84A6-4E77-458E-8AF9-112074A58E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECDB569-23DE-4616-BBE6-2BCB60EBE3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Material</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t xml:space="preserve"> PT26 IM PT2 SAN</t>
+  </si>
+  <si>
+    <t>algo</t>
   </si>
 </sst>
 </file>
@@ -253,10 +256,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,25 +574,25 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>11001</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="C2" s="3">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11003</v>
+        <v>11001</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -597,10 +603,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11007</v>
+        <v>11003</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -611,10 +617,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11009</v>
+        <v>11007</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -625,24 +631,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>11038</v>
+        <v>11009</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>11099</v>
+        <v>11038</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -653,164 +659,164 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>11137</v>
+        <v>11099</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11154</v>
+        <v>11137</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11489</v>
+        <v>11154</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11558</v>
+        <v>11489</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11560</v>
+        <v>11558</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11647</v>
+        <v>11560</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11649</v>
+        <v>11647</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11654</v>
+        <v>11649</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11655</v>
+        <v>11654</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11656</v>
+        <v>11655</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>11664</v>
+        <v>11656</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>11665</v>
+        <v>11664</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -821,24 +827,24 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>11795</v>
+        <v>11665</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>11806</v>
+        <v>11795</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -849,94 +855,94 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>11808</v>
+        <v>11806</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>11867</v>
+        <v>11808</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>11974</v>
+        <v>11867</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>11978</v>
+        <v>11974</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>11993</v>
+        <v>11978</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>11994</v>
+        <v>11993</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>11996</v>
+        <v>11994</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -947,321 +953,363 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>12003</v>
+        <v>11996</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>110</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>12008</v>
+        <v>12003</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D30">
-        <v>60</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>12019</v>
+        <v>12008</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>12035</v>
+        <v>12019</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32">
-        <v>360</v>
+        <v>100</v>
       </c>
       <c r="D32">
-        <v>360</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>12037</v>
+        <v>12035</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D33">
-        <v>160</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>12038</v>
+        <v>12037</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34">
-        <v>300</v>
+        <v>160</v>
       </c>
       <c r="D34">
-        <v>300</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>12039</v>
+        <v>12038</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D35">
-        <v>180</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>12040</v>
+        <v>12039</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>12041</v>
+        <v>12039</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>12042</v>
+        <v>12040</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>12058</v>
+        <v>12041</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="D39">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>12062</v>
+        <v>12042</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>12063</v>
+        <v>12058</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>12064</v>
+        <v>12062</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>12086</v>
+        <v>12063</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D43">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>12088</v>
+        <v>12064</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D44">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>12089</v>
+        <v>12086</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>12090</v>
+        <v>11111</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>12131</v>
+        <v>12088</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D47">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>12132</v>
+        <v>12089</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C48">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>12177</v>
+        <v>12090</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C49">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D49">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
+        <v>12131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+      <c r="D50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>12132</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>12177</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>55</v>
+      </c>
+      <c r="D52">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>12217</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>52</v>
       </c>
-      <c r="C50">
+      <c r="C53">
         <v>8</v>
       </c>
-      <c r="D50">
+      <c r="D53">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>